<commit_message>
home page test cases
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Project\Learning-hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20496" windowHeight="7764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="RM" sheetId="2" r:id="rId2"/>
+    <sheet name="HM" sheetId="3" r:id="rId2"/>
+    <sheet name="RM" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -212,12 +213,27 @@
   <si>
     <t>The system submitted the new account normally without giving any errors</t>
   </si>
+  <si>
+    <t>HM_Bug_001</t>
+  </si>
+  <si>
+    <t>HM_11</t>
+  </si>
+  <si>
+    <t>the " home " button is not directing to the home page</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3-find the navigation bar on the top of the page
+4- click on " home " button</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +279,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +303,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -391,6 +420,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,20 +719,20 @@
       <selection activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.26953125" customWidth="1"/>
-    <col min="3" max="3" width="45.7265625" customWidth="1"/>
-    <col min="4" max="4" width="34.54296875" customWidth="1"/>
-    <col min="5" max="6" width="32.26953125" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.21875" customWidth="1"/>
+    <col min="3" max="3" width="45.77734375" customWidth="1"/>
+    <col min="4" max="4" width="34.5546875" customWidth="1"/>
+    <col min="5" max="6" width="32.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="27.77734375" customWidth="1"/>
     <col min="9" max="9" width="41" customWidth="1"/>
-    <col min="10" max="10" width="35.54296875" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -738,7 +780,7 @@
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" s="9" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
@@ -786,7 +828,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -815,13 +857,13 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -829,24 +871,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="25" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="11" max="16384" width="8.77734375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="20" customFormat="1" ht="37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" s="20" customFormat="1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -894,7 +1032,7 @@
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:26" s="22" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" s="22" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>28</v>
       </c>
@@ -942,7 +1080,7 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:26" s="22" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" s="22" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
@@ -990,7 +1128,7 @@
       <c r="Y3" s="21"/>
       <c r="Z3" s="21"/>
     </row>
-    <row r="4" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -1022,7 +1160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
@@ -1054,7 +1192,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
@@ -1086,10 +1224,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish home page test case and bug report
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20496" windowHeight="7764" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20496" windowHeight="7764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,241 @@
 2- Run the project on Google Chrome or Firefox browsers
 3-find the navigation bar on the top of the page
 4- click on " home " button</t>
+  </si>
+  <si>
+    <t>HM_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional </t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " My profile " button</t>
+  </si>
+  <si>
+    <t>the" My Profile " button direct the user to the his/her Profile page</t>
+  </si>
+  <si>
+    <t>Erro page appears</t>
+  </si>
+  <si>
+    <t>HM_18</t>
+  </si>
+  <si>
+    <t>check that " English " is the only language
+used in writing articles</t>
+  </si>
+  <si>
+    <t>HM_19</t>
+  </si>
+  <si>
+    <t>HM_20</t>
+  </si>
+  <si>
+    <t>check that vedio format is MP4</t>
+  </si>
+  <si>
+    <t>check that system reject other vedio formats</t>
+  </si>
+  <si>
+    <t>check that vedio size is unlimited</t>
+  </si>
+  <si>
+    <t>HM_21</t>
+  </si>
+  <si>
+    <t>check that audio format is MP3</t>
+  </si>
+  <si>
+    <t>HM_22</t>
+  </si>
+  <si>
+    <t>check that system reject other audio formats</t>
+  </si>
+  <si>
+    <t>HM_23</t>
+  </si>
+  <si>
+    <t>HM_24</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " + " button
+7- write the tittle and field of the article
+8- upload an article in English language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " + " button
+7- write the tittle and field of the article
+8- upload an article in Arabic language
+</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+1-find the navigation bar on the top of the page
+2- click on " + " button
+3- write the tittle and field of the article
+ 4- upload an article in MPv format
+5- upload the vedio with size 500 MB</t>
+  </si>
+  <si>
+    <t>1- log in with valid username
+and password
+2- Direct to " Home " page
+3- get notification already
+4-find the " Notification " button bar on the top of the page
+5- click on " Notification " button</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5- get notification already
+6-find the " Notification " button bar on the top of the page
+7- notice the " Notification " button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " + " button
+7- write the tittle and field of the article
+8- upload an article in WAV format
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+1-find the navigation bar on the top of the page
+2- click on " + " button
+3- write the tittle and field of the article
+ 4- upload an article in MP3 format
+</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " + " button
+7- write the tittle and field of the article
+8- upload an article in MPV format</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Direct to " Home " page
+5-find the navigation bar on the top of the page
+6- click on " + " button
+7- write the tittle and field of the article 
+8- upload an article in MP4 format</t>
+  </si>
+  <si>
+    <t>the " My Profile " button is not directing to the Profile page</t>
+  </si>
+  <si>
+    <t>the color of " notification " doesn't change by new notifications</t>
+  </si>
+  <si>
+    <t>the " Notification " button is not directing to the notification page</t>
+  </si>
+  <si>
+    <t>sustem accept the upload process</t>
+  </si>
+  <si>
+    <t>system reject the upload process</t>
+  </si>
+  <si>
+    <t>system accepty vedio with any size</t>
+  </si>
+  <si>
+    <t>system accept the MP3 format</t>
+  </si>
+  <si>
+    <t>system reject the WAV format</t>
+  </si>
+  <si>
+    <t>the notification button is red</t>
+  </si>
+  <si>
+    <t>button not working</t>
+  </si>
+  <si>
+    <t>the " Notification " button direct the user to the Notification page</t>
+  </si>
+  <si>
+    <t>HM_Bug_02</t>
+  </si>
+  <si>
+    <t>HM_Bug_01</t>
+  </si>
+  <si>
+    <t>HM_Bug_03</t>
+  </si>
+  <si>
+    <t>HM_Bug_04</t>
+  </si>
+  <si>
+    <t>HM_Bug_05</t>
+  </si>
+  <si>
+    <t>HM_Bug_06</t>
+  </si>
+  <si>
+    <t>HM_Bug_07</t>
+  </si>
+  <si>
+    <t>HM_Bug_08</t>
+  </si>
+  <si>
+    <t>HM_Bug_09</t>
+  </si>
+  <si>
+    <t>HM_Bug_10</t>
+  </si>
+  <si>
+    <t>HM_26</t>
+  </si>
+  <si>
+    <t>HM_25</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>meduim</t>
   </si>
 </sst>
 </file>
@@ -355,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -420,18 +655,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,16 +1144,16 @@
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="25" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -901,7 +1163,7 @@
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -926,18 +1188,18 @@
     </row>
     <row r="2" spans="1:11" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>58</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -956,6 +1218,449 @@
         <v>41</v>
       </c>
       <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="138" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E13" s="37"/>
+    </row>
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E14" s="37"/>
+    </row>
+    <row r="15" spans="1:11" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:11" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E18" s="30"/>
+    </row>
+    <row r="19" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E21" s="30"/>
+    </row>
+    <row r="22" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E35" s="31"/>
+    </row>
+    <row r="36" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E37" s="31"/>
+    </row>
+    <row r="38" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E41" s="31"/>
+    </row>
+    <row r="42" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E42" s="31"/>
+    </row>
+    <row r="43" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E43" s="31"/>
+    </row>
+    <row r="44" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E44" s="31"/>
+    </row>
+    <row r="45" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E45" s="31"/>
+    </row>
+    <row r="46" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E46" s="31"/>
+    </row>
+    <row r="47" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E47" s="31"/>
+    </row>
+    <row r="48" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E50" s="31"/>
+    </row>
+    <row r="51" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E51" s="31"/>
+    </row>
+    <row r="52" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E52" s="31"/>
+    </row>
+    <row r="53" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E53" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish home page bug report
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20496" windowHeight="7764" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20496" windowHeight="7764" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -462,6 +462,15 @@
   </si>
   <si>
     <t>meduim</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Designed By</t>
+  </si>
+  <si>
+    <t>NADA</t>
   </si>
 </sst>
 </file>
@@ -590,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -694,6 +703,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1151,9 +1166,11 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,9 +1201,14 @@
       <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="19"/>
-    </row>
-    <row r="2" spans="1:11" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="K1" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="27" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>98</v>
       </c>
@@ -1217,9 +1239,12 @@
       <c r="J2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="138" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" s="33" customFormat="1" ht="138" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
@@ -1250,8 +1275,12 @@
       <c r="J3" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="K3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>99</v>
       </c>
@@ -1282,8 +1311,12 @@
       <c r="J4" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="K4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>55</v>
       </c>
@@ -1314,8 +1347,12 @@
       <c r="J5" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="K5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" s="33" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>100</v>
       </c>
@@ -1346,8 +1383,12 @@
       <c r="J6" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="K6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" s="33" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>101</v>
       </c>
@@ -1378,8 +1419,12 @@
       <c r="J7" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="K7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" s="33" customFormat="1" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>102</v>
       </c>
@@ -1410,8 +1455,12 @@
       <c r="J8" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="K8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>103</v>
       </c>
@@ -1442,8 +1491,12 @@
       <c r="J9" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
+      <c r="K9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" s="33" customFormat="1" ht="207" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>104</v>
       </c>
@@ -1474,8 +1527,12 @@
       <c r="J10" s="34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="K10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" s="33" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>105</v>
       </c>
@@ -1506,8 +1563,12 @@
       <c r="J11" s="34" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="K11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" s="33" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>106</v>
       </c>
@@ -1538,17 +1599,21 @@
       <c r="J12" s="34" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="K12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="E14" s="37"/>
     </row>
-    <row r="15" spans="1:11" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="E15" s="30"/>
     </row>
-    <row r="16" spans="1:11" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="E16" s="30"/>
     </row>
     <row r="17" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update testcases with testcases of category module
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\ProjectManagement\project\Learning-hub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="HM" sheetId="3" r:id="rId2"/>
-    <sheet name="RM" sheetId="2" r:id="rId3"/>
+    <sheet name="CATMODULE" sheetId="4" r:id="rId2"/>
+    <sheet name="HM" sheetId="3" r:id="rId3"/>
+    <sheet name="RM" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -472,12 +473,50 @@
   <si>
     <t>NADA</t>
   </si>
+  <si>
+    <t>Cat_Module_05</t>
+  </si>
+  <si>
+    <t>Cat_ModuleBUG_05</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>check the status of followed category when 
+the user logged out and logged in again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- log in with valid username
+and password
+4- Open" Category " page
+5-follow specific category
+6-Log out form tha account
+7-log in again
+8-check that you are still following the same category
+</t>
+  </si>
+  <si>
+    <t>when the user logout and logged in again he is still following the category</t>
+  </si>
+  <si>
+    <t>the user isnot still following 
+the category</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>wafaa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +564,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -599,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -709,6 +755,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1150,8 +1205,374 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="27" customFormat="1" ht="336" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E13" s="37"/>
+    </row>
+    <row r="14" spans="1:12" s="33" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E14" s="37"/>
+    </row>
+    <row r="15" spans="1:12" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:12" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E18" s="30"/>
+    </row>
+    <row r="19" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="5:5" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E21" s="30"/>
+    </row>
+    <row r="22" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E23" s="31"/>
+    </row>
+    <row r="24" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E35" s="31"/>
+    </row>
+    <row r="36" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E37" s="31"/>
+    </row>
+    <row r="38" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E38" s="31"/>
+    </row>
+    <row r="39" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E41" s="31"/>
+    </row>
+    <row r="42" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E42" s="31"/>
+    </row>
+    <row r="43" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E43" s="31"/>
+    </row>
+    <row r="44" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E44" s="31"/>
+    </row>
+    <row r="45" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E45" s="31"/>
+    </row>
+    <row r="46" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E46" s="31"/>
+    </row>
+    <row r="47" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E47" s="31"/>
+    </row>
+    <row r="48" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E48" s="31"/>
+    </row>
+    <row r="49" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E49" s="31"/>
+    </row>
+    <row r="50" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E50" s="31"/>
+    </row>
+    <row r="51" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E51" s="31"/>
+    </row>
+    <row r="52" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E52" s="31"/>
+    </row>
+    <row r="53" spans="5:5" s="32" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="E53" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +2154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>

</xml_diff>

<commit_message>
add name to bug report
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="20496" windowHeight="7764" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20496" windowHeight="7764" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="CATMODULE" sheetId="4" r:id="rId2"/>
-    <sheet name="HM" sheetId="3" r:id="rId3"/>
+    <sheet name="HM-Nada" sheetId="3" r:id="rId3"/>
     <sheet name="RM" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add my bug reports
</commit_message>
<xml_diff>
--- a/Testing/Bug_Report.xlsx
+++ b/Testing/Bug_Report.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA_project\Learning-hub\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI subjects\software project management\project 3\Learning-hub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20496" windowHeight="7764" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="20496" windowHeight="7764" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="CATMODULE" sheetId="4" r:id="rId2"/>
+    <sheet name="CAT_MODULE" sheetId="4" r:id="rId2"/>
     <sheet name="HM-Nada" sheetId="3" r:id="rId3"/>
     <sheet name="RM" sheetId="2" r:id="rId4"/>
+    <sheet name="login_module_Ragab" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -439,12 +440,94 @@
   <si>
     <t>blocked</t>
   </si>
+  <si>
+    <t>lhub_login_1</t>
+  </si>
+  <si>
+    <t>lhub_login_bug_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,   click on "Login" button
+4- type in "USERNAME" field as in test data
+5- type in "PASSWORD" field as in test data
+6- click on "Login" button
+</t>
+  </si>
+  <si>
+    <t>user will be redirected to the home page and the "test39" is placed at the left side of the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password is incorrect although there  test data is stored in the database 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opened </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciritcal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">login functionality is not working with a valid user name and password , although thy are stored in the database of the website </t>
+  </si>
+  <si>
+    <t xml:space="preserve">functional </t>
+  </si>
+  <si>
+    <t>lhub_login_bug_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- open the website project with visual studio
+2- run the project without debugging either on google chrome or firefox web browser
+3- after the website is opened in firefox or google chrome web browser,  click on "Login" button
+4- click on "forget your password" button
+5- enter a valid email address as provided in test data
+6- click on "send" button 
+7-  enter a valid email address as provided in test data 
+8 - enter a valid new password as provided in test data
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is redirected to “reset password “ page </t>
+  </si>
+  <si>
+    <t>after entering a valid user name and clicking on  "forget your password" button , an error message appears " password is required " , and I cannot redirect to next page which I can enter a valid emaill</t>
+  </si>
+  <si>
+    <t>lhub_login_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is not redirected to "forget password" page when click on "forget you password link to provide a valid email address to recover  his password  </t>
+  </si>
+  <si>
+    <t>test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+user name: test39
+password :  TesMe39$#
+new password:  NewMe39$#
+email: learninghub@gmail.com
+FIRST NAME : power
+LAST NAME:  learners
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+user name: test39
+password :  TesMe39$#
+email: learninghub@gmail.com
+FIRST NAME : power
+LAST NAME:  learners
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +587,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,6 +638,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -570,10 +685,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -690,8 +806,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -972,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1496,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1939,7 +2074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2205,4 +2342,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="50" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="70.88671875" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="42" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+    </row>
+    <row r="2" spans="1:27" s="47" customFormat="1" ht="198" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="47" customFormat="1" ht="252" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>